<commit_message>
completed telek-math analysis and updated spreadsheet
</commit_message>
<xml_diff>
--- a/Spreadsheet/Testing_Project_Book.xlsx
+++ b/Spreadsheet/Testing_Project_Book.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://kennesawedu-my.sharepoint.com/personal/jharr651_students_kennesaw_edu/Documents/Microsoft Teams Chat Files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="760" documentId="8_{0075BCC8-5893-458B-9267-D692CF2E0844}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{37010E90-0B37-4DF6-8FA4-BE8562BB932F}"/>
+  <xr:revisionPtr revIDLastSave="1396" documentId="8_{0075BCC8-5893-458B-9267-D692CF2E0844}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E7C7BB7C-B6A7-47DA-8188-54939B87FEF6}"/>
   <bookViews>
-    <workbookView xWindow="18120" yWindow="-16350" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="1" xr2:uid="{626E3A53-FCA0-448E-8C24-39C3188B5282}"/>
+    <workbookView xWindow="18120" yWindow="-16350" windowWidth="29040" windowHeight="15840" firstSheet="3" activeTab="3" xr2:uid="{626E3A53-FCA0-448E-8C24-39C3188B5282}"/>
   </bookViews>
   <sheets>
     <sheet name="JSON-java" sheetId="1" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1936" uniqueCount="710">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1956" uniqueCount="718">
   <si>
     <t>Test Suite</t>
   </si>
@@ -1876,6 +1876,30 @@
   </si>
   <si>
     <t>testTopDownMergeSort</t>
+  </si>
+  <si>
+    <t>plain</t>
+  </si>
+  <si>
+    <t>containers</t>
+  </si>
+  <si>
+    <t>colors</t>
+  </si>
+  <si>
+    <t>arrayref</t>
+  </si>
+  <si>
+    <t>utils</t>
+  </si>
+  <si>
+    <t>special</t>
+  </si>
+  <si>
+    <t>core</t>
+  </si>
+  <si>
+    <t>advanced</t>
   </si>
   <si>
     <t>com.telek.tests.dists.ChiSqDistTest</t>
@@ -7569,8 +7593,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08833A34-32DC-4145-AE02-42649B2D339F}">
   <dimension ref="A1:Q59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
-      <selection activeCell="A59" sqref="A59"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.45"/>
@@ -12860,1030 +12884,3044 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3EAFE1BE-8FF1-42D0-B3F9-29F870221CF2}">
-  <dimension ref="A1:F158"/>
+  <dimension ref="A1:M158"/>
   <sheetViews>
-    <sheetView topLeftCell="A41" workbookViewId="0">
-      <selection activeCell="E49" sqref="E49"/>
+    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="D71" sqref="D71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.45"/>
   <cols>
-    <col min="1" max="1" width="46.42578125" customWidth="1"/>
+    <col min="1" max="1" width="46.28515625" customWidth="1"/>
     <col min="2" max="2" width="40.7109375" customWidth="1"/>
     <col min="3" max="3" width="20.5703125" customWidth="1"/>
-    <col min="4" max="4" width="24.140625" customWidth="1"/>
-    <col min="5" max="5" width="23" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" customWidth="1"/>
+    <col min="5" max="5" width="10.5703125" customWidth="1"/>
+    <col min="6" max="6" width="10.85546875" customWidth="1"/>
+    <col min="7" max="7" width="12.28515625" customWidth="1"/>
+    <col min="8" max="8" width="8" customWidth="1"/>
+    <col min="9" max="9" width="9.5703125" customWidth="1"/>
+    <col min="10" max="10" width="10.42578125" customWidth="1"/>
+    <col min="11" max="11" width="12.5703125" customWidth="1"/>
+    <col min="12" max="12" width="23" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="3" t="s">
+    <row r="1" spans="1:13" ht="15">
+      <c r="A1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="6" t="s">
+        <v>610</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>611</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>612</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>613</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>614</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>615</v>
+      </c>
+      <c r="J1" s="6" t="s">
+        <v>616</v>
+      </c>
+      <c r="K1" s="6" t="s">
+        <v>617</v>
+      </c>
+      <c r="L1" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="M1" s="10" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" ht="15">
+      <c r="A2" t="s">
+        <v>618</v>
+      </c>
+      <c r="B2" t="s">
+        <v>619</v>
+      </c>
+      <c r="C2">
+        <v>252</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>160</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
+      <c r="J2">
+        <v>1</v>
+      </c>
+      <c r="K2">
+        <v>91</v>
+      </c>
+      <c r="L2">
+        <v>85</v>
+      </c>
+      <c r="M2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" ht="15">
+      <c r="A3" t="s">
+        <v>618</v>
+      </c>
+      <c r="B3" t="s">
+        <v>620</v>
+      </c>
+      <c r="C3">
+        <v>257</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>166</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+      <c r="J3">
+        <v>1</v>
+      </c>
+      <c r="K3">
+        <v>90</v>
+      </c>
+      <c r="L3">
+        <v>202</v>
+      </c>
+      <c r="M3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" ht="15">
+      <c r="A4" t="s">
+        <v>618</v>
+      </c>
+      <c r="B4" t="s">
+        <v>621</v>
+      </c>
+      <c r="C4">
+        <v>159</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>157</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
+      <c r="J4">
+        <v>0</v>
+      </c>
+      <c r="K4">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="L4">
+        <v>1</v>
+      </c>
+      <c r="M4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" ht="15">
+      <c r="A5" t="s">
+        <v>618</v>
+      </c>
+      <c r="B5" t="s">
+        <v>622</v>
+      </c>
+      <c r="C5">
+        <v>152</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>149</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+      <c r="J5">
+        <v>0</v>
+      </c>
+      <c r="K5">
+        <v>3</v>
+      </c>
+      <c r="L5">
+        <v>1</v>
+      </c>
+      <c r="M5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" ht="15">
+      <c r="A6" t="s">
+        <v>623</v>
+      </c>
+      <c r="B6" t="s">
+        <v>624</v>
+      </c>
+      <c r="C6">
+        <v>22</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>10</v>
+      </c>
+      <c r="I6">
+        <v>0</v>
+      </c>
+      <c r="J6">
+        <v>0</v>
+      </c>
+      <c r="K6">
+        <v>12</v>
+      </c>
+      <c r="L6">
+        <v>49</v>
+      </c>
+      <c r="M6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" ht="15">
+      <c r="A7" t="s">
+        <v>625</v>
+      </c>
+      <c r="B7" t="s">
+        <v>619</v>
+      </c>
+      <c r="C7">
+        <f>SUM(D7:K7)</f>
+        <v>239</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>213</v>
+      </c>
+      <c r="I7">
+        <v>0</v>
+      </c>
+      <c r="J7">
+        <v>0</v>
+      </c>
+      <c r="K7">
+        <v>26</v>
+      </c>
+      <c r="L7">
+        <v>2</v>
+      </c>
+      <c r="M7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" ht="15">
+      <c r="A8" t="s">
+        <v>625</v>
+      </c>
+      <c r="B8" t="s">
+        <v>620</v>
+      </c>
+      <c r="C8">
+        <f>SUM(D8:K8)</f>
+        <v>240</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <v>213</v>
+      </c>
+      <c r="I8">
+        <v>0</v>
+      </c>
+      <c r="J8">
+        <v>0</v>
+      </c>
+      <c r="K8">
+        <v>27</v>
+      </c>
+      <c r="L8">
+        <v>126</v>
+      </c>
+      <c r="M8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" ht="15">
+      <c r="A9" t="s">
+        <v>625</v>
+      </c>
+      <c r="B9" t="s">
+        <v>621</v>
+      </c>
+      <c r="C9">
+        <f>SUM(D9:K9)</f>
+        <v>148</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9">
+        <v>145</v>
+      </c>
+      <c r="I9">
+        <v>0</v>
+      </c>
+      <c r="J9">
+        <v>0</v>
+      </c>
+      <c r="K9">
+        <v>3</v>
+      </c>
+      <c r="L9">
+        <v>28</v>
+      </c>
+      <c r="M9" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" ht="15">
+      <c r="A10" t="s">
+        <v>625</v>
+      </c>
+      <c r="B10" t="s">
+        <v>622</v>
+      </c>
+      <c r="C10">
+        <f>SUM(D10:K10)</f>
+        <v>122</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <v>119</v>
+      </c>
+      <c r="I10">
+        <v>0</v>
+      </c>
+      <c r="J10">
+        <v>0</v>
+      </c>
+      <c r="K10">
+        <v>3</v>
+      </c>
+      <c r="L10">
+        <v>22</v>
+      </c>
+      <c r="M10" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" ht="15">
+      <c r="A11" t="s">
+        <v>626</v>
+      </c>
+      <c r="B11" t="s">
+        <v>627</v>
+      </c>
+      <c r="C11">
+        <f>SUM(D11:K11)</f>
+        <v>11</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <v>10</v>
+      </c>
+      <c r="I11">
+        <v>0</v>
+      </c>
+      <c r="J11">
+        <v>0</v>
+      </c>
+      <c r="K11">
+        <v>1</v>
+      </c>
+      <c r="L11">
+        <v>3</v>
+      </c>
+      <c r="M11" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" ht="15">
+      <c r="A12" t="s">
+        <v>626</v>
+      </c>
+      <c r="B12" t="s">
+        <v>628</v>
+      </c>
+      <c r="C12">
+        <f>SUM(D12:K12)</f>
+        <v>19</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+      <c r="H12">
+        <v>15</v>
+      </c>
+      <c r="I12">
+        <v>0</v>
+      </c>
+      <c r="J12">
+        <v>0</v>
+      </c>
+      <c r="K12">
         <v>4</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="L12">
+        <v>17</v>
+      </c>
+      <c r="M12" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" ht="15">
+      <c r="A13" t="s">
+        <v>626</v>
+      </c>
+      <c r="B13" t="s">
+        <v>629</v>
+      </c>
+      <c r="C13">
+        <f>SUM(D13:K13)</f>
+        <v>18</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+      <c r="G13">
+        <v>0</v>
+      </c>
+      <c r="H13">
+        <v>10</v>
+      </c>
+      <c r="I13">
+        <v>0</v>
+      </c>
+      <c r="J13">
+        <v>0</v>
+      </c>
+      <c r="K13">
+        <v>8</v>
+      </c>
+      <c r="L13">
+        <v>88</v>
+      </c>
+      <c r="M13" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" ht="15">
+      <c r="A14" t="s">
+        <v>626</v>
+      </c>
+      <c r="B14" t="s">
+        <v>630</v>
+      </c>
+      <c r="C14">
+        <f>SUM(D14:K14)</f>
+        <v>14</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
+      <c r="G14">
+        <v>0</v>
+      </c>
+      <c r="H14">
+        <v>10</v>
+      </c>
+      <c r="I14">
+        <v>0</v>
+      </c>
+      <c r="J14">
+        <v>0</v>
+      </c>
+      <c r="K14">
+        <v>4</v>
+      </c>
+      <c r="L14">
+        <v>13</v>
+      </c>
+      <c r="M14" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" ht="15">
+      <c r="A15" t="s">
+        <v>626</v>
+      </c>
+      <c r="B15" t="s">
+        <v>631</v>
+      </c>
+      <c r="C15">
+        <f>SUM(D15:K15)</f>
+        <v>14</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
+      <c r="F15">
+        <v>0</v>
+      </c>
+      <c r="G15">
+        <v>0</v>
+      </c>
+      <c r="H15">
+        <v>10</v>
+      </c>
+      <c r="I15">
+        <v>0</v>
+      </c>
+      <c r="J15">
+        <v>0</v>
+      </c>
+      <c r="K15">
+        <v>4</v>
+      </c>
+      <c r="L15">
+        <v>6</v>
+      </c>
+      <c r="M15" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" ht="15">
+      <c r="A16" t="s">
+        <v>626</v>
+      </c>
+      <c r="B16" t="s">
+        <v>622</v>
+      </c>
+      <c r="C16">
+        <f>SUM(D16:K16)</f>
+        <v>8</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+      <c r="E16">
+        <v>0</v>
+      </c>
+      <c r="F16">
+        <v>0</v>
+      </c>
+      <c r="G16">
+        <v>0</v>
+      </c>
+      <c r="H16">
+        <v>7</v>
+      </c>
+      <c r="I16">
+        <v>0</v>
+      </c>
+      <c r="J16">
+        <v>0</v>
+      </c>
+      <c r="K16">
+        <v>1</v>
+      </c>
+      <c r="L16">
+        <v>6</v>
+      </c>
+      <c r="M16" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" ht="15">
+      <c r="A17" t="s">
+        <v>632</v>
+      </c>
+      <c r="B17" t="s">
+        <v>633</v>
+      </c>
+      <c r="C17">
+        <f>SUM(D17:K17)</f>
+        <v>84</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
+      <c r="E17">
+        <v>0</v>
+      </c>
+      <c r="F17">
+        <v>0</v>
+      </c>
+      <c r="G17">
+        <v>0</v>
+      </c>
+      <c r="H17">
+        <v>7</v>
+      </c>
+      <c r="I17">
+        <v>0</v>
+      </c>
+      <c r="J17">
+        <v>77</v>
+      </c>
+      <c r="K17">
+        <v>0</v>
+      </c>
+      <c r="L17">
+        <v>7</v>
+      </c>
+      <c r="M17" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" ht="15">
+      <c r="A18" t="s">
+        <v>632</v>
+      </c>
+      <c r="B18" t="s">
+        <v>634</v>
+      </c>
+      <c r="C18">
+        <f>SUM(D18:K18)</f>
+        <v>126</v>
+      </c>
+      <c r="D18">
+        <v>0</v>
+      </c>
+      <c r="E18">
+        <v>0</v>
+      </c>
+      <c r="F18">
+        <v>0</v>
+      </c>
+      <c r="G18">
+        <v>0</v>
+      </c>
+      <c r="H18">
+        <v>7</v>
+      </c>
+      <c r="I18">
+        <v>0</v>
+      </c>
+      <c r="J18">
+        <v>119</v>
+      </c>
+      <c r="K18">
+        <v>0</v>
+      </c>
+      <c r="L18">
+        <v>14</v>
+      </c>
+      <c r="M18" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" ht="15">
+      <c r="A19" t="s">
+        <v>635</v>
+      </c>
+      <c r="B19" t="s">
+        <v>636</v>
+      </c>
+      <c r="C19">
+        <f>SUM(D19:K19)</f>
+        <v>175</v>
+      </c>
+      <c r="D19">
+        <v>0</v>
+      </c>
+      <c r="E19">
+        <v>0</v>
+      </c>
+      <c r="F19">
+        <v>0</v>
+      </c>
+      <c r="G19">
+        <v>0</v>
+      </c>
+      <c r="H19">
+        <v>7</v>
+      </c>
+      <c r="I19">
+        <v>0</v>
+      </c>
+      <c r="J19">
+        <v>168</v>
+      </c>
+      <c r="K19">
+        <v>0</v>
+      </c>
+      <c r="L19">
+        <v>11</v>
+      </c>
+      <c r="M19" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" ht="15">
+      <c r="A20" t="s">
+        <v>635</v>
+      </c>
+      <c r="B20" t="s">
+        <v>637</v>
+      </c>
+      <c r="C20">
+        <f>SUM(D20:K20)</f>
+        <v>93</v>
+      </c>
+      <c r="D20">
+        <v>0</v>
+      </c>
+      <c r="E20">
+        <v>0</v>
+      </c>
+      <c r="F20">
+        <v>0</v>
+      </c>
+      <c r="G20">
+        <v>0</v>
+      </c>
+      <c r="H20">
+        <v>8</v>
+      </c>
+      <c r="I20">
+        <v>0</v>
+      </c>
+      <c r="J20">
+        <v>85</v>
+      </c>
+      <c r="K20">
+        <v>0</v>
+      </c>
+      <c r="L20">
+        <v>1</v>
+      </c>
+      <c r="M20" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" ht="15">
+      <c r="A21" t="s">
+        <v>638</v>
+      </c>
+      <c r="B21" t="s">
+        <v>639</v>
+      </c>
+      <c r="C21">
+        <f>SUM(D21:K21)</f>
+        <v>67</v>
+      </c>
+      <c r="D21">
+        <v>0</v>
+      </c>
+      <c r="E21">
+        <v>0</v>
+      </c>
+      <c r="F21">
+        <v>0</v>
+      </c>
+      <c r="G21">
+        <v>0</v>
+      </c>
+      <c r="I21">
+        <v>0</v>
+      </c>
+      <c r="J21">
+        <v>67</v>
+      </c>
+      <c r="K21">
+        <v>0</v>
+      </c>
+      <c r="L21">
+        <v>2</v>
+      </c>
+      <c r="M21" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" ht="15">
+      <c r="A22" t="s">
+        <v>640</v>
+      </c>
+      <c r="B22" t="s">
+        <v>641</v>
+      </c>
+      <c r="C22">
+        <f>SUM(D22:K22)</f>
+        <v>50</v>
+      </c>
+      <c r="D22">
+        <v>0</v>
+      </c>
+      <c r="E22">
+        <v>0</v>
+      </c>
+      <c r="F22">
+        <v>0</v>
+      </c>
+      <c r="G22">
+        <v>0</v>
+      </c>
+      <c r="H22">
+        <v>7</v>
+      </c>
+      <c r="I22">
+        <v>0</v>
+      </c>
+      <c r="J22">
+        <v>43</v>
+      </c>
+      <c r="K22">
+        <v>0</v>
+      </c>
+      <c r="L22">
+        <v>4</v>
+      </c>
+      <c r="M22" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" ht="15">
+      <c r="A23" t="s">
+        <v>642</v>
+      </c>
+      <c r="B23" t="s">
+        <v>643</v>
+      </c>
+      <c r="C23">
+        <f>SUM(D23:K23)</f>
+        <v>24</v>
+      </c>
+      <c r="D23">
+        <v>0</v>
+      </c>
+      <c r="E23">
+        <v>0</v>
+      </c>
+      <c r="F23">
+        <v>0</v>
+      </c>
+      <c r="G23">
+        <v>0</v>
+      </c>
+      <c r="H23">
+        <v>7</v>
+      </c>
+      <c r="I23">
+        <v>0</v>
+      </c>
+      <c r="J23">
+        <v>17</v>
+      </c>
+      <c r="K23">
+        <v>0</v>
+      </c>
+      <c r="L23">
+        <v>12</v>
+      </c>
+      <c r="M23" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" ht="15">
+      <c r="A24" t="s">
+        <v>644</v>
+      </c>
+      <c r="B24" t="s">
+        <v>645</v>
+      </c>
+      <c r="C24">
+        <f>SUM(D24:K24)</f>
+        <v>18</v>
+      </c>
+      <c r="D24">
+        <v>0</v>
+      </c>
+      <c r="E24">
+        <v>0</v>
+      </c>
+      <c r="F24">
+        <v>0</v>
+      </c>
+      <c r="G24">
+        <v>0</v>
+      </c>
+      <c r="H24">
+        <v>7</v>
+      </c>
+      <c r="I24">
+        <v>0</v>
+      </c>
+      <c r="J24">
+        <v>11</v>
+      </c>
+      <c r="K24">
+        <v>0</v>
+      </c>
+      <c r="L24">
+        <v>10</v>
+      </c>
+      <c r="M24" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" ht="15">
+      <c r="A25" t="s">
+        <v>646</v>
+      </c>
+      <c r="B25" t="s">
+        <v>647</v>
+      </c>
+      <c r="C25">
+        <f>SUM(D25:K25)</f>
+        <v>25</v>
+      </c>
+      <c r="D25">
+        <v>0</v>
+      </c>
+      <c r="E25">
+        <v>0</v>
+      </c>
+      <c r="F25">
+        <v>0</v>
+      </c>
+      <c r="G25">
+        <v>0</v>
+      </c>
+      <c r="H25">
+        <v>7</v>
+      </c>
+      <c r="I25">
+        <v>0</v>
+      </c>
+      <c r="J25">
+        <v>18</v>
+      </c>
+      <c r="K25">
+        <v>0</v>
+      </c>
+      <c r="L25">
+        <v>4</v>
+      </c>
+      <c r="M25" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" ht="15">
+      <c r="A26" t="s">
+        <v>648</v>
+      </c>
+      <c r="B26" t="s">
+        <v>649</v>
+      </c>
+      <c r="C26">
+        <f>SUM(D26:K26)</f>
+        <v>44</v>
+      </c>
+      <c r="D26">
+        <v>0</v>
+      </c>
+      <c r="E26">
+        <v>0</v>
+      </c>
+      <c r="F26">
+        <v>0</v>
+      </c>
+      <c r="G26">
+        <v>0</v>
+      </c>
+      <c r="H26">
+        <v>7</v>
+      </c>
+      <c r="I26">
+        <v>0</v>
+      </c>
+      <c r="J26">
+        <v>37</v>
+      </c>
+      <c r="K26">
+        <v>0</v>
+      </c>
+      <c r="L26">
+        <v>2</v>
+      </c>
+      <c r="M26" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" ht="15">
+      <c r="A27" t="s">
+        <v>650</v>
+      </c>
+      <c r="B27" t="s">
+        <v>651</v>
+      </c>
+      <c r="C27">
+        <f>SUM(D27:K27)</f>
+        <v>106</v>
+      </c>
+      <c r="D27">
+        <v>0</v>
+      </c>
+      <c r="E27">
+        <v>4</v>
+      </c>
+      <c r="F27">
+        <v>0</v>
+      </c>
+      <c r="G27">
+        <v>0</v>
+      </c>
+      <c r="H27">
+        <v>1</v>
+      </c>
+      <c r="I27">
+        <v>0</v>
+      </c>
+      <c r="J27">
+        <v>101</v>
+      </c>
+      <c r="K27">
+        <v>0</v>
+      </c>
+      <c r="L27">
+        <v>16</v>
+      </c>
+      <c r="M27" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" ht="15">
+      <c r="A28" t="s">
+        <v>650</v>
+      </c>
+      <c r="B28" t="s">
+        <v>652</v>
+      </c>
+      <c r="C28">
+        <f>SUM(D28:K28)</f>
+        <v>124</v>
+      </c>
+      <c r="D28">
+        <v>0</v>
+      </c>
+      <c r="E28">
+        <v>19</v>
+      </c>
+      <c r="F28">
+        <v>0</v>
+      </c>
+      <c r="G28">
+        <v>0</v>
+      </c>
+      <c r="H28">
+        <v>1</v>
+      </c>
+      <c r="I28">
+        <v>0</v>
+      </c>
+      <c r="J28">
+        <v>104</v>
+      </c>
+      <c r="K28">
+        <v>0</v>
+      </c>
+      <c r="L28">
+        <v>4</v>
+      </c>
+      <c r="M28" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" ht="15">
+      <c r="A29" t="s">
+        <v>650</v>
+      </c>
+      <c r="B29" t="s">
+        <v>653</v>
+      </c>
+      <c r="C29">
+        <f>SUM(D29:K29)</f>
+        <v>8</v>
+      </c>
+      <c r="D29">
+        <v>0</v>
+      </c>
+      <c r="E29">
+        <v>1</v>
+      </c>
+      <c r="F29">
+        <v>0</v>
+      </c>
+      <c r="G29">
+        <v>0</v>
+      </c>
+      <c r="H29">
+        <v>0</v>
+      </c>
+      <c r="I29">
+        <v>0</v>
+      </c>
+      <c r="J29">
+        <v>7</v>
+      </c>
+      <c r="K29">
+        <v>0</v>
+      </c>
+      <c r="L29">
+        <v>5</v>
+      </c>
+      <c r="M29" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" ht="15">
+      <c r="A30" t="s">
+        <v>654</v>
+      </c>
+      <c r="B30" t="s">
+        <v>655</v>
+      </c>
+      <c r="C30">
+        <f>SUM(D30:K30)</f>
+        <v>103</v>
+      </c>
+      <c r="D30">
+        <v>0</v>
+      </c>
+      <c r="E30">
+        <v>4</v>
+      </c>
+      <c r="F30">
+        <v>0</v>
+      </c>
+      <c r="G30">
+        <v>0</v>
+      </c>
+      <c r="H30">
+        <v>0</v>
+      </c>
+      <c r="I30">
+        <v>0</v>
+      </c>
+      <c r="J30">
+        <v>99</v>
+      </c>
+      <c r="K30">
+        <v>0</v>
+      </c>
+      <c r="L30">
+        <v>6</v>
+      </c>
+      <c r="M30" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" ht="15">
+      <c r="A31" t="s">
+        <v>656</v>
+      </c>
+      <c r="B31" t="s">
+        <v>657</v>
+      </c>
+      <c r="C31">
+        <f>SUM(D31:K31)</f>
+        <v>26</v>
+      </c>
+      <c r="D31">
+        <v>0</v>
+      </c>
+      <c r="E31">
+        <v>0</v>
+      </c>
+      <c r="F31">
+        <v>0</v>
+      </c>
+      <c r="G31">
+        <v>0</v>
+      </c>
+      <c r="H31">
+        <v>7</v>
+      </c>
+      <c r="I31">
+        <v>0</v>
+      </c>
+      <c r="J31">
+        <v>19</v>
+      </c>
+      <c r="K31">
+        <v>0</v>
+      </c>
+      <c r="L31">
+        <v>2</v>
+      </c>
+      <c r="M31" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" ht="15">
+      <c r="A32" t="s">
+        <v>658</v>
+      </c>
+      <c r="B32" t="s">
+        <v>659</v>
+      </c>
+      <c r="C32">
+        <f>SUM(D32:K32)</f>
+        <v>38</v>
+      </c>
+      <c r="D32">
+        <v>0</v>
+      </c>
+      <c r="E32">
+        <v>0</v>
+      </c>
+      <c r="F32">
+        <v>0</v>
+      </c>
+      <c r="G32">
+        <v>0</v>
+      </c>
+      <c r="H32">
+        <v>8</v>
+      </c>
+      <c r="I32">
+        <v>0</v>
+      </c>
+      <c r="J32">
+        <v>30</v>
+      </c>
+      <c r="K32">
+        <v>0</v>
+      </c>
+      <c r="L32">
+        <v>4</v>
+      </c>
+      <c r="M32" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" ht="15">
+      <c r="A33" t="s">
+        <v>660</v>
+      </c>
+      <c r="B33" t="s">
+        <v>661</v>
+      </c>
+      <c r="C33">
+        <f>SUM(D33:K33)</f>
+        <v>17</v>
+      </c>
+      <c r="D33">
+        <v>0</v>
+      </c>
+      <c r="E33">
+        <v>0</v>
+      </c>
+      <c r="F33">
+        <v>0</v>
+      </c>
+      <c r="G33">
+        <v>0</v>
+      </c>
+      <c r="H33">
+        <v>8</v>
+      </c>
+      <c r="I33">
+        <v>0</v>
+      </c>
+      <c r="J33">
+        <v>9</v>
+      </c>
+      <c r="K33">
+        <v>0</v>
+      </c>
+      <c r="L33">
+        <v>5</v>
+      </c>
+      <c r="M33" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" ht="15">
+      <c r="A34" t="s">
+        <v>662</v>
+      </c>
+      <c r="B34" t="s">
+        <v>663</v>
+      </c>
+      <c r="C34">
+        <f>SUM(D34:K34)</f>
+        <v>249</v>
+      </c>
+      <c r="D34">
+        <v>0</v>
+      </c>
+      <c r="F34">
+        <v>0</v>
+      </c>
+      <c r="G34">
+        <v>0</v>
+      </c>
+      <c r="H34">
+        <v>118</v>
+      </c>
+      <c r="I34">
+        <v>0</v>
+      </c>
+      <c r="J34">
+        <v>14</v>
+      </c>
+      <c r="K34">
+        <v>117</v>
+      </c>
+      <c r="L34">
+        <v>12</v>
+      </c>
+      <c r="M34" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" ht="15">
+      <c r="A35" t="s">
+        <v>662</v>
+      </c>
+      <c r="B35" t="s">
+        <v>664</v>
+      </c>
+      <c r="C35">
+        <f>SUM(D35:K35)</f>
+        <v>279</v>
+      </c>
+      <c r="D35">
+        <v>0</v>
+      </c>
+      <c r="E35">
+        <v>7</v>
+      </c>
+      <c r="F35">
+        <v>0</v>
+      </c>
+      <c r="G35">
+        <v>4</v>
+      </c>
+      <c r="H35">
+        <v>118</v>
+      </c>
+      <c r="I35">
+        <v>0</v>
+      </c>
+      <c r="J35">
+        <v>1</v>
+      </c>
+      <c r="K35">
+        <v>149</v>
+      </c>
+      <c r="L35">
+        <v>9</v>
+      </c>
+      <c r="M35" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" ht="15">
+      <c r="A36" t="s">
+        <v>662</v>
+      </c>
+      <c r="B36" t="s">
+        <v>665</v>
+      </c>
+      <c r="C36">
+        <f>SUM(D36:K36)</f>
+        <v>350</v>
+      </c>
+      <c r="D36">
+        <v>0</v>
+      </c>
+      <c r="E36">
+        <v>15</v>
+      </c>
+      <c r="F36">
+        <v>0</v>
+      </c>
+      <c r="G36">
+        <v>16</v>
+      </c>
+      <c r="H36">
+        <v>118</v>
+      </c>
+      <c r="I36">
+        <v>0</v>
+      </c>
+      <c r="J36">
+        <v>14</v>
+      </c>
+      <c r="K36">
+        <v>187</v>
+      </c>
+      <c r="L36">
+        <v>6</v>
+      </c>
+      <c r="M36" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" ht="15">
+      <c r="A37" t="s">
+        <v>666</v>
+      </c>
+      <c r="B37" t="s">
+        <v>667</v>
+      </c>
+      <c r="C37">
+        <f>SUM(D37:K37)</f>
+        <v>340</v>
+      </c>
+      <c r="D37">
+        <v>0</v>
+      </c>
+      <c r="E37">
+        <v>11</v>
+      </c>
+      <c r="F37">
+        <v>0</v>
+      </c>
+      <c r="G37">
+        <v>4</v>
+      </c>
+      <c r="H37">
+        <v>196</v>
+      </c>
+      <c r="I37">
+        <v>0</v>
+      </c>
+      <c r="J37">
+        <v>9</v>
+      </c>
+      <c r="K37">
+        <v>120</v>
+      </c>
+      <c r="L37">
+        <v>4</v>
+      </c>
+      <c r="M37" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" ht="15">
+      <c r="A38" t="s">
+        <v>666</v>
+      </c>
+      <c r="B38" t="s">
+        <v>668</v>
+      </c>
+      <c r="C38">
+        <f>SUM(D38:K38)</f>
+        <v>133</v>
+      </c>
+      <c r="D38">
+        <v>0</v>
+      </c>
+      <c r="E38">
+        <v>11</v>
+      </c>
+      <c r="F38">
+        <v>0</v>
+      </c>
+      <c r="G38">
+        <v>4</v>
+      </c>
+      <c r="H38">
+        <v>16</v>
+      </c>
+      <c r="I38">
+        <v>0</v>
+      </c>
+      <c r="J38">
+        <v>9</v>
+      </c>
+      <c r="K38">
+        <v>93</v>
+      </c>
+      <c r="L38">
+        <v>3</v>
+      </c>
+      <c r="M38" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" ht="15">
+      <c r="A39" t="s">
+        <v>666</v>
+      </c>
+      <c r="B39" t="s">
+        <v>669</v>
+      </c>
+      <c r="C39">
+        <f>SUM(D39:K39)</f>
+        <v>341</v>
+      </c>
+      <c r="D39">
+        <v>0</v>
+      </c>
+      <c r="E39">
+        <v>11</v>
+      </c>
+      <c r="F39">
+        <v>0</v>
+      </c>
+      <c r="G39">
+        <v>4</v>
+      </c>
+      <c r="H39">
+        <v>136</v>
+      </c>
+      <c r="I39">
+        <v>0</v>
+      </c>
+      <c r="J39">
+        <v>10</v>
+      </c>
+      <c r="K39">
+        <v>180</v>
+      </c>
+      <c r="L39">
+        <v>3</v>
+      </c>
+      <c r="M39" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" ht="15">
+      <c r="A40" t="s">
+        <v>666</v>
+      </c>
+      <c r="B40" t="s">
+        <v>670</v>
+      </c>
+      <c r="C40">
+        <f>SUM(D40:K40)</f>
+        <v>363</v>
+      </c>
+      <c r="D40">
+        <v>4</v>
+      </c>
+      <c r="E40">
+        <v>7</v>
+      </c>
+      <c r="F40">
+        <v>0</v>
+      </c>
+      <c r="G40">
+        <v>5</v>
+      </c>
+      <c r="H40">
+        <v>138</v>
+      </c>
+      <c r="I40">
+        <v>0</v>
+      </c>
+      <c r="J40">
+        <v>5</v>
+      </c>
+      <c r="K40">
+        <v>204</v>
+      </c>
+      <c r="L40">
+        <v>1</v>
+      </c>
+      <c r="M40" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" ht="15">
+      <c r="A41" t="s">
+        <v>671</v>
+      </c>
+      <c r="B41" t="s">
+        <v>672</v>
+      </c>
+      <c r="C41">
+        <f>SUM(D41:K41)</f>
+        <v>136</v>
+      </c>
+      <c r="D41">
+        <v>0</v>
+      </c>
+      <c r="E41">
+        <v>4</v>
+      </c>
+      <c r="F41">
+        <v>0</v>
+      </c>
+      <c r="G41">
+        <v>4</v>
+      </c>
+      <c r="H41">
+        <v>16</v>
+      </c>
+      <c r="I41">
+        <v>0</v>
+      </c>
+      <c r="J41">
+        <v>9</v>
+      </c>
+      <c r="K41">
+        <v>103</v>
+      </c>
+      <c r="L41">
+        <v>5</v>
+      </c>
+      <c r="M41" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" ht="15">
+      <c r="A42" t="s">
+        <v>671</v>
+      </c>
+      <c r="B42" t="s">
+        <v>673</v>
+      </c>
+      <c r="C42">
+        <f>SUM(D42:K42)</f>
+        <v>135</v>
+      </c>
+      <c r="D42">
+        <v>0</v>
+      </c>
+      <c r="E42">
+        <v>4</v>
+      </c>
+      <c r="F42">
+        <v>0</v>
+      </c>
+      <c r="G42">
+        <v>4</v>
+      </c>
+      <c r="H42">
+        <v>16</v>
+      </c>
+      <c r="I42">
+        <v>0</v>
+      </c>
+      <c r="J42">
+        <v>9</v>
+      </c>
+      <c r="K42">
+        <v>102</v>
+      </c>
+      <c r="L42">
+        <v>1</v>
+      </c>
+      <c r="M42" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" ht="15">
+      <c r="A43" t="s">
+        <v>671</v>
+      </c>
+      <c r="B43" t="s">
+        <v>674</v>
+      </c>
+      <c r="C43">
+        <f>SUM(D43:K43)</f>
+        <v>343</v>
+      </c>
+      <c r="D43">
+        <v>0</v>
+      </c>
+      <c r="E43">
+        <v>4</v>
+      </c>
+      <c r="F43">
+        <v>0</v>
+      </c>
+      <c r="G43">
+        <v>4</v>
+      </c>
+      <c r="H43">
+        <v>188</v>
+      </c>
+      <c r="I43">
+        <v>0</v>
+      </c>
+      <c r="J43">
+        <v>9</v>
+      </c>
+      <c r="K43">
+        <v>138</v>
+      </c>
+      <c r="L43">
+        <v>5</v>
+      </c>
+      <c r="M43" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" ht="15">
+      <c r="A44" t="s">
+        <v>675</v>
+      </c>
+      <c r="B44" t="s">
+        <v>676</v>
+      </c>
+      <c r="C44">
+        <f>SUM(D44:K44)</f>
+        <v>111</v>
+      </c>
+      <c r="D44">
+        <v>4</v>
+      </c>
+      <c r="E44">
+        <v>7</v>
+      </c>
+      <c r="F44">
+        <v>0</v>
+      </c>
+      <c r="G44">
+        <v>5</v>
+      </c>
+      <c r="H44">
+        <v>8</v>
+      </c>
+      <c r="I44">
+        <v>0</v>
+      </c>
+      <c r="J44">
+        <v>0</v>
+      </c>
+      <c r="K44">
+        <v>87</v>
+      </c>
+      <c r="L44">
+        <v>3</v>
+      </c>
+      <c r="M44" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" ht="15">
+      <c r="A45" t="s">
+        <v>675</v>
+      </c>
+      <c r="B45" t="s">
+        <v>677</v>
+      </c>
+      <c r="C45">
+        <f>SUM(D45:K45)</f>
+        <v>111</v>
+      </c>
+      <c r="D45">
+        <v>0</v>
+      </c>
+      <c r="E45">
+        <v>8</v>
+      </c>
+      <c r="F45">
+        <v>0</v>
+      </c>
+      <c r="G45">
+        <v>4</v>
+      </c>
+      <c r="H45">
+        <v>8</v>
+      </c>
+      <c r="I45">
+        <v>0</v>
+      </c>
+      <c r="J45">
+        <v>0</v>
+      </c>
+      <c r="K45">
+        <v>91</v>
+      </c>
+      <c r="L45">
+        <v>1</v>
+      </c>
+      <c r="M45" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" ht="15">
+      <c r="A46" t="s">
+        <v>675</v>
+      </c>
+      <c r="B46" t="s">
+        <v>678</v>
+      </c>
+      <c r="C46">
+        <f>SUM(D46:K46)</f>
+        <v>117</v>
+      </c>
+      <c r="D46">
+        <v>4</v>
+      </c>
+      <c r="E46">
+        <v>15</v>
+      </c>
+      <c r="F46">
+        <v>0</v>
+      </c>
+      <c r="G46">
+        <v>9</v>
+      </c>
+      <c r="H46">
+        <v>8</v>
+      </c>
+      <c r="I46">
+        <v>0</v>
+      </c>
+      <c r="J46">
+        <v>0</v>
+      </c>
+      <c r="K46">
+        <v>81</v>
+      </c>
+      <c r="L46">
+        <v>12</v>
+      </c>
+      <c r="M46" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13" ht="15">
+      <c r="A47" t="s">
+        <v>675</v>
+      </c>
+      <c r="B47" t="s">
+        <v>679</v>
+      </c>
+      <c r="C47">
+        <f>SUM(D47:K47)</f>
+        <v>123</v>
+      </c>
+      <c r="D47">
+        <v>0</v>
+      </c>
+      <c r="E47">
+        <v>24</v>
+      </c>
+      <c r="F47">
+        <v>0</v>
+      </c>
+      <c r="G47">
+        <v>4</v>
+      </c>
+      <c r="H47">
+        <v>8</v>
+      </c>
+      <c r="I47">
+        <v>0</v>
+      </c>
+      <c r="J47">
+        <v>0</v>
+      </c>
+      <c r="K47">
+        <v>87</v>
+      </c>
+      <c r="L47">
+        <v>5421</v>
+      </c>
+      <c r="M47" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13" ht="15">
+      <c r="A48" t="s">
+        <v>675</v>
+      </c>
+      <c r="B48" t="s">
+        <v>680</v>
+      </c>
+      <c r="C48">
+        <f>SUM(D48:K48)</f>
+        <v>124</v>
+      </c>
+      <c r="D48">
+        <v>0</v>
+      </c>
+      <c r="E48">
+        <v>8</v>
+      </c>
+      <c r="F48">
+        <v>0</v>
+      </c>
+      <c r="G48">
+        <v>4</v>
+      </c>
+      <c r="H48">
+        <v>8</v>
+      </c>
+      <c r="I48">
+        <v>0</v>
+      </c>
+      <c r="J48">
+        <v>0</v>
+      </c>
+      <c r="K48">
+        <v>104</v>
+      </c>
+      <c r="L48">
+        <v>2</v>
+      </c>
+      <c r="M48" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="49" spans="1:13" ht="15">
+      <c r="A49" t="s">
+        <v>675</v>
+      </c>
+      <c r="B49" t="s">
+        <v>681</v>
+      </c>
+      <c r="C49">
+        <f>SUM(D49:K49)</f>
+        <v>109</v>
+      </c>
+      <c r="D49">
+        <v>0</v>
+      </c>
+      <c r="E49">
+        <v>32</v>
+      </c>
+      <c r="F49">
+        <v>0</v>
+      </c>
+      <c r="G49">
+        <v>12</v>
+      </c>
+      <c r="H49">
+        <v>7</v>
+      </c>
+      <c r="I49">
+        <v>0</v>
+      </c>
+      <c r="J49">
+        <v>0</v>
+      </c>
+      <c r="K49">
+        <v>58</v>
+      </c>
+      <c r="L49">
+        <v>360</v>
+      </c>
+      <c r="M49" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13" ht="15">
+      <c r="A50" t="s">
+        <v>682</v>
+      </c>
+      <c r="B50" t="s">
+        <v>683</v>
+      </c>
+      <c r="C50">
+        <f>SUM(D50:K50)</f>
+        <v>71</v>
+      </c>
+      <c r="D50">
+        <v>0</v>
+      </c>
+      <c r="E50">
+        <v>11</v>
+      </c>
+      <c r="F50">
+        <v>0</v>
+      </c>
+      <c r="G50">
+        <v>12</v>
+      </c>
+      <c r="H50">
+        <v>7</v>
+      </c>
+      <c r="I50">
+        <v>0</v>
+      </c>
+      <c r="J50">
+        <v>0</v>
+      </c>
+      <c r="K50">
+        <v>41</v>
+      </c>
+      <c r="L50">
+        <v>227</v>
+      </c>
+      <c r="M50" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="51" spans="1:13" ht="15">
+      <c r="A51" t="s">
+        <v>682</v>
+      </c>
+      <c r="B51" t="s">
+        <v>684</v>
+      </c>
+      <c r="C51">
+        <f>SUM(D51:K51)</f>
+        <v>130</v>
+      </c>
+      <c r="D51">
+        <v>4</v>
+      </c>
+      <c r="E51">
+        <v>11</v>
+      </c>
+      <c r="F51">
+        <v>0</v>
+      </c>
+      <c r="G51">
+        <v>5</v>
+      </c>
+      <c r="H51">
+        <v>70</v>
+      </c>
+      <c r="I51">
+        <v>0</v>
+      </c>
+      <c r="J51">
+        <v>0</v>
+      </c>
+      <c r="K51">
+        <v>40</v>
+      </c>
+      <c r="L51">
+        <v>899</v>
+      </c>
+      <c r="M51" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13" ht="15">
+      <c r="A52" t="s">
+        <v>682</v>
+      </c>
+      <c r="B52" t="s">
+        <v>685</v>
+      </c>
+      <c r="C52">
+        <f>SUM(D52:K52)</f>
+        <v>93</v>
+      </c>
+      <c r="D52">
+        <v>0</v>
+      </c>
+      <c r="E52">
+        <v>11</v>
+      </c>
+      <c r="F52">
+        <v>0</v>
+      </c>
+      <c r="G52">
+        <v>16</v>
+      </c>
+      <c r="I52">
+        <v>0</v>
+      </c>
+      <c r="J52">
+        <v>0</v>
+      </c>
+      <c r="K52">
+        <v>66</v>
+      </c>
+      <c r="L52">
+        <v>4</v>
+      </c>
+      <c r="M52" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="53" spans="1:13" ht="15">
+      <c r="A53" t="s">
+        <v>682</v>
+      </c>
+      <c r="B53" t="s">
+        <v>686</v>
+      </c>
+      <c r="C53">
+        <f>SUM(D53:K53)</f>
+        <v>64</v>
+      </c>
+      <c r="D53">
+        <v>0</v>
+      </c>
+      <c r="E53">
+        <v>14</v>
+      </c>
+      <c r="F53">
+        <v>0</v>
+      </c>
+      <c r="G53">
+        <v>4</v>
+      </c>
+      <c r="H53">
+        <v>7</v>
+      </c>
+      <c r="I53">
+        <v>0</v>
+      </c>
+      <c r="J53">
+        <v>0</v>
+      </c>
+      <c r="K53">
+        <v>39</v>
+      </c>
+      <c r="L53">
+        <v>12337</v>
+      </c>
+      <c r="M53" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="54" spans="1:13" ht="15">
+      <c r="A54" t="s">
+        <v>687</v>
+      </c>
+      <c r="B54" t="s">
+        <v>688</v>
+      </c>
+      <c r="C54">
+        <f>SUM(D54:K54)</f>
+        <v>532</v>
+      </c>
+      <c r="D54">
+        <v>0</v>
+      </c>
+      <c r="E54">
+        <v>11</v>
+      </c>
+      <c r="F54">
+        <v>0</v>
+      </c>
+      <c r="G54">
+        <v>4</v>
+      </c>
+      <c r="H54">
+        <v>264</v>
+      </c>
+      <c r="I54">
+        <v>0</v>
+      </c>
+      <c r="J54">
+        <v>1</v>
+      </c>
+      <c r="K54">
+        <v>252</v>
+      </c>
+      <c r="L54">
+        <v>501</v>
+      </c>
+      <c r="M54" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="55" spans="1:13" ht="15">
+      <c r="A55" t="s">
+        <v>689</v>
+      </c>
+      <c r="B55" t="s">
+        <v>690</v>
+      </c>
+      <c r="C55">
+        <f>SUM(D55:K55)</f>
+        <v>406</v>
+      </c>
+      <c r="D55">
+        <v>0</v>
+      </c>
+      <c r="E55">
+        <v>21</v>
+      </c>
+      <c r="F55">
+        <v>0</v>
+      </c>
+      <c r="G55">
+        <v>8</v>
+      </c>
+      <c r="H55">
+        <v>218</v>
+      </c>
+      <c r="I55">
+        <v>0</v>
+      </c>
+      <c r="J55">
+        <v>1</v>
+      </c>
+      <c r="K55">
+        <v>158</v>
+      </c>
+      <c r="L55">
+        <v>74</v>
+      </c>
+      <c r="M55" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="56" spans="1:13" ht="15">
+      <c r="A56" t="s">
+        <v>689</v>
+      </c>
+      <c r="B56" t="s">
+        <v>691</v>
+      </c>
+      <c r="C56">
+        <f>SUM(D56:K56)</f>
+        <v>149</v>
+      </c>
+      <c r="D56">
+        <v>0</v>
+      </c>
+      <c r="E56">
+        <v>21</v>
+      </c>
+      <c r="F56">
+        <v>0</v>
+      </c>
+      <c r="G56">
+        <v>8</v>
+      </c>
+      <c r="H56">
+        <v>7</v>
+      </c>
+      <c r="I56">
+        <v>0</v>
+      </c>
+      <c r="J56">
+        <v>1</v>
+      </c>
+      <c r="K56">
+        <v>112</v>
+      </c>
+      <c r="L56">
+        <v>1</v>
+      </c>
+      <c r="M56" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="57" spans="1:13" ht="15">
+      <c r="A57" t="s">
+        <v>692</v>
+      </c>
+      <c r="B57" t="s">
+        <v>693</v>
+      </c>
+      <c r="C57">
+        <f>SUM(D57:K57)</f>
+        <v>47</v>
+      </c>
+      <c r="D57">
+        <v>0</v>
+      </c>
+      <c r="E57">
+        <v>0</v>
+      </c>
+      <c r="F57">
+        <v>0</v>
+      </c>
+      <c r="G57">
+        <v>0</v>
+      </c>
+      <c r="H57">
+        <v>0</v>
+      </c>
+      <c r="I57">
+        <v>0</v>
+      </c>
+      <c r="J57">
+        <v>4</v>
+      </c>
+      <c r="K57">
+        <v>43</v>
+      </c>
+      <c r="L57">
+        <v>2</v>
+      </c>
+      <c r="M57" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="58" spans="1:13" ht="15">
+      <c r="A58" t="s">
+        <v>692</v>
+      </c>
+      <c r="B58" t="s">
+        <v>694</v>
+      </c>
+      <c r="C58">
+        <f>SUM(D58:K58)</f>
+        <v>42</v>
+      </c>
+      <c r="D58">
+        <v>0</v>
+      </c>
+      <c r="E58">
+        <v>0</v>
+      </c>
+      <c r="F58">
+        <v>0</v>
+      </c>
+      <c r="G58">
+        <v>0</v>
+      </c>
+      <c r="H58">
+        <v>0</v>
+      </c>
+      <c r="I58">
+        <v>0</v>
+      </c>
+      <c r="J58">
+        <v>4</v>
+      </c>
+      <c r="K58">
+        <v>38</v>
+      </c>
+      <c r="L58">
+        <v>1</v>
+      </c>
+      <c r="M58" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="59" spans="1:13" ht="15">
+      <c r="A59" t="s">
+        <v>692</v>
+      </c>
+      <c r="B59" t="s">
+        <v>695</v>
+      </c>
+      <c r="C59">
+        <f>SUM(D59:K59)</f>
+        <v>42</v>
+      </c>
+      <c r="D59">
+        <v>0</v>
+      </c>
+      <c r="E59">
+        <v>0</v>
+      </c>
+      <c r="F59">
+        <v>0</v>
+      </c>
+      <c r="G59">
+        <v>0</v>
+      </c>
+      <c r="H59">
+        <v>0</v>
+      </c>
+      <c r="I59">
+        <v>0</v>
+      </c>
+      <c r="J59">
+        <v>4</v>
+      </c>
+      <c r="K59">
+        <v>38</v>
+      </c>
+      <c r="L59">
+        <v>12</v>
+      </c>
+      <c r="M59" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="60" spans="1:13" ht="15">
+      <c r="A60" t="s">
+        <v>696</v>
+      </c>
+      <c r="B60" t="s">
+        <v>697</v>
+      </c>
+      <c r="C60">
+        <f>SUM(D60:K60)</f>
+        <v>387</v>
+      </c>
+      <c r="D60">
+        <v>4</v>
+      </c>
+      <c r="E60">
+        <v>0</v>
+      </c>
+      <c r="F60">
+        <v>0</v>
+      </c>
+      <c r="G60">
+        <v>20</v>
+      </c>
+      <c r="H60">
+        <v>191</v>
+      </c>
+      <c r="I60">
+        <v>0</v>
+      </c>
+      <c r="J60">
+        <v>23</v>
+      </c>
+      <c r="K60">
+        <v>149</v>
+      </c>
+      <c r="L60">
+        <v>7</v>
+      </c>
+      <c r="M60" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="61" spans="1:13" ht="15">
+      <c r="A61" t="s">
+        <v>698</v>
+      </c>
+      <c r="B61" t="s">
+        <v>699</v>
+      </c>
+      <c r="C61">
+        <f>SUM(D61:K61)</f>
+        <v>503</v>
+      </c>
+      <c r="D61">
+        <v>0</v>
+      </c>
+      <c r="E61">
+        <v>0</v>
+      </c>
+      <c r="F61">
+        <v>0</v>
+      </c>
+      <c r="G61">
+        <v>5</v>
+      </c>
+      <c r="H61">
+        <v>213</v>
+      </c>
+      <c r="I61">
+        <v>0</v>
+      </c>
+      <c r="J61">
+        <v>33</v>
+      </c>
+      <c r="K61">
+        <v>252</v>
+      </c>
+      <c r="L61">
+        <v>2</v>
+      </c>
+      <c r="M61" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="62" spans="1:13" ht="15">
+      <c r="A62" t="s">
+        <v>700</v>
+      </c>
+      <c r="B62" t="s">
+        <v>701</v>
+      </c>
+      <c r="C62">
+        <f>SUM(D62:K62)</f>
+        <v>75</v>
+      </c>
+      <c r="D62">
+        <v>0</v>
+      </c>
+      <c r="E62">
+        <v>0</v>
+      </c>
+      <c r="F62">
+        <v>0</v>
+      </c>
+      <c r="G62">
+        <v>75</v>
+      </c>
+      <c r="H62">
+        <v>0</v>
+      </c>
+      <c r="I62">
+        <v>0</v>
+      </c>
+      <c r="J62">
+        <v>0</v>
+      </c>
+      <c r="K62">
+        <v>0</v>
+      </c>
+      <c r="L62">
+        <v>46</v>
+      </c>
+      <c r="M62" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="63" spans="1:13" ht="15">
+      <c r="A63" t="s">
+        <v>700</v>
+      </c>
+      <c r="B63" t="s">
+        <v>702</v>
+      </c>
+      <c r="C63">
+        <f>SUM(D63:K63)</f>
+        <v>46</v>
+      </c>
+      <c r="D63">
+        <v>4</v>
+      </c>
+      <c r="E63">
+        <v>0</v>
+      </c>
+      <c r="F63">
+        <v>0</v>
+      </c>
+      <c r="G63">
+        <v>42</v>
+      </c>
+      <c r="H63">
+        <v>0</v>
+      </c>
+      <c r="I63">
+        <v>0</v>
+      </c>
+      <c r="J63">
+        <v>0</v>
+      </c>
+      <c r="K63">
+        <v>0</v>
+      </c>
+      <c r="L63">
+        <v>20</v>
+      </c>
+      <c r="M63" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="64" spans="1:13" ht="15">
+      <c r="A64" t="s">
+        <v>703</v>
+      </c>
+      <c r="B64" t="s">
+        <v>704</v>
+      </c>
+      <c r="C64">
+        <f>SUM(D64:K64)</f>
+        <v>19</v>
+      </c>
+      <c r="D64">
+        <v>0</v>
+      </c>
+      <c r="E64">
+        <v>0</v>
+      </c>
+      <c r="F64">
+        <v>19</v>
+      </c>
+      <c r="G64">
+        <v>0</v>
+      </c>
+      <c r="H64">
+        <v>0</v>
+      </c>
+      <c r="I64">
+        <v>0</v>
+      </c>
+      <c r="J64">
+        <v>0</v>
+      </c>
+      <c r="K64">
+        <v>0</v>
+      </c>
+      <c r="L64">
+        <v>2</v>
+      </c>
+      <c r="M64" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="65" spans="1:13" ht="15">
+      <c r="A65" t="s">
+        <v>705</v>
+      </c>
+      <c r="B65" t="s">
+        <v>706</v>
+      </c>
+      <c r="C65">
+        <f>SUM(D65:K65)</f>
+        <v>93</v>
+      </c>
+      <c r="D65">
+        <v>2</v>
+      </c>
+      <c r="E65">
+        <v>0</v>
+      </c>
+      <c r="F65">
+        <v>0</v>
+      </c>
+      <c r="G65">
+        <v>0</v>
+      </c>
+      <c r="H65">
+        <v>0</v>
+      </c>
+      <c r="I65">
+        <v>18</v>
+      </c>
+      <c r="J65">
+        <v>10</v>
+      </c>
+      <c r="K65">
+        <v>63</v>
+      </c>
+      <c r="L65">
+        <v>328</v>
+      </c>
+      <c r="M65" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="66" spans="1:13" ht="15">
+      <c r="A66" t="s">
+        <v>707</v>
+      </c>
+      <c r="B66" t="s">
+        <v>708</v>
+      </c>
+      <c r="C66">
+        <f>SUM(D66:K66)</f>
+        <v>49</v>
+      </c>
+      <c r="D66">
+        <v>0</v>
+      </c>
+      <c r="E66">
+        <v>0</v>
+      </c>
+      <c r="F66">
+        <v>0</v>
+      </c>
+      <c r="G66">
+        <v>0</v>
+      </c>
+      <c r="H66">
+        <v>1</v>
+      </c>
+      <c r="I66">
+        <v>48</v>
+      </c>
+      <c r="J66">
+        <v>0</v>
+      </c>
+      <c r="K66">
+        <v>0</v>
+      </c>
+      <c r="L66">
+        <v>1</v>
+      </c>
+      <c r="M66" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="67" spans="1:13" ht="15">
+      <c r="A67" t="s">
+        <v>709</v>
+      </c>
+      <c r="B67" t="s">
+        <v>710</v>
+      </c>
+      <c r="C67">
+        <f>SUM(D67:K67)</f>
+        <v>19</v>
+      </c>
+      <c r="D67">
+        <v>0</v>
+      </c>
+      <c r="E67">
+        <v>0</v>
+      </c>
+      <c r="F67">
+        <v>0</v>
+      </c>
+      <c r="G67">
+        <v>0</v>
+      </c>
+      <c r="H67">
+        <v>0</v>
+      </c>
+      <c r="I67">
+        <v>19</v>
+      </c>
+      <c r="J67">
+        <v>0</v>
+      </c>
+      <c r="K67">
+        <v>0</v>
+      </c>
+      <c r="L67">
+        <v>2</v>
+      </c>
+      <c r="M67" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="68" spans="1:13" ht="15">
+      <c r="A68" t="s">
+        <v>711</v>
+      </c>
+      <c r="B68" t="s">
+        <v>712</v>
+      </c>
+      <c r="C68">
+        <f>SUM(D68:K68)</f>
+        <v>155</v>
+      </c>
+      <c r="D68">
+        <v>0</v>
+      </c>
+      <c r="E68">
+        <v>0</v>
+      </c>
+      <c r="F68">
+        <v>0</v>
+      </c>
+      <c r="G68">
+        <v>4</v>
+      </c>
+      <c r="H68">
+        <v>7</v>
+      </c>
+      <c r="I68">
+        <v>82</v>
+      </c>
+      <c r="J68">
+        <v>62</v>
+      </c>
+      <c r="K68">
+        <v>0</v>
+      </c>
+      <c r="L68">
+        <v>5</v>
+      </c>
+      <c r="M68" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="69" spans="1:13" ht="15">
+      <c r="A69" t="s">
+        <v>713</v>
+      </c>
+      <c r="B69" t="s">
+        <v>714</v>
+      </c>
+      <c r="C69">
+        <f>SUM(D69:K69)</f>
+        <v>4</v>
+      </c>
+      <c r="D69">
+        <v>0</v>
+      </c>
+      <c r="E69">
+        <v>4</v>
+      </c>
+      <c r="F69">
+        <v>0</v>
+      </c>
+      <c r="G69">
+        <v>0</v>
+      </c>
+      <c r="H69">
+        <v>0</v>
+      </c>
+      <c r="I69">
+        <v>0</v>
+      </c>
+      <c r="J69">
+        <v>0</v>
+      </c>
+      <c r="K69">
+        <v>0</v>
+      </c>
+      <c r="L69">
+        <v>2</v>
+      </c>
+      <c r="M69" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="70" spans="1:13" ht="15">
+      <c r="A70" t="s">
+        <v>713</v>
+      </c>
+      <c r="B70" t="s">
+        <v>715</v>
+      </c>
+      <c r="C70">
+        <f>SUM(D70:K70)</f>
+        <v>18</v>
+      </c>
+      <c r="D70">
+        <v>0</v>
+      </c>
+      <c r="E70">
+        <v>18</v>
+      </c>
+      <c r="F70">
+        <v>0</v>
+      </c>
+      <c r="G70">
+        <v>0</v>
+      </c>
+      <c r="H70">
+        <v>0</v>
+      </c>
+      <c r="I70">
+        <v>0</v>
+      </c>
+      <c r="J70">
+        <v>0</v>
+      </c>
+      <c r="K70">
+        <v>0</v>
+      </c>
+      <c r="L70">
+        <v>1</v>
+      </c>
+      <c r="M70" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="71" spans="1:13" ht="15">
+      <c r="A71" t="s">
+        <v>716</v>
+      </c>
+      <c r="B71" t="s">
+        <v>717</v>
+      </c>
+      <c r="C71">
+        <f>SUM(D71:K71)</f>
+        <v>105</v>
+      </c>
+      <c r="D71">
+        <v>0</v>
+      </c>
+      <c r="E71">
+        <v>0</v>
+      </c>
+      <c r="F71">
+        <v>0</v>
+      </c>
+      <c r="G71">
+        <v>0</v>
+      </c>
+      <c r="H71">
+        <v>105</v>
+      </c>
+      <c r="I71">
+        <v>0</v>
+      </c>
+      <c r="J71">
+        <v>0</v>
+      </c>
+      <c r="K71">
+        <v>0</v>
+      </c>
+      <c r="L71">
+        <v>1</v>
+      </c>
+      <c r="M71" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="72" spans="1:13" ht="15">
+      <c r="A72" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B72" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C72" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D72" s="6" t="s">
+        <v>610</v>
+      </c>
+      <c r="E72" s="6" t="s">
+        <v>611</v>
+      </c>
+      <c r="F72" s="6" t="s">
+        <v>612</v>
+      </c>
+      <c r="G72" s="6" t="s">
+        <v>613</v>
+      </c>
+      <c r="H72" s="6" t="s">
+        <v>614</v>
+      </c>
+      <c r="I72" s="6" t="s">
+        <v>615</v>
+      </c>
+      <c r="J72" s="6" t="s">
+        <v>616</v>
+      </c>
+      <c r="K72" s="6" t="s">
+        <v>617</v>
+      </c>
+      <c r="L72" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="M72" s="10" t="s">
         <v>346</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15">
-      <c r="A2" t="s">
-        <v>610</v>
-      </c>
-      <c r="B2" t="s">
-        <v>611</v>
-      </c>
-      <c r="E2">
-        <v>85</v>
-      </c>
-      <c r="F2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="15">
-      <c r="A3" t="s">
-        <v>610</v>
-      </c>
-      <c r="B3" t="s">
-        <v>612</v>
-      </c>
-      <c r="E3">
-        <v>202</v>
-      </c>
-      <c r="F3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="15">
-      <c r="A4" t="s">
-        <v>610</v>
-      </c>
-      <c r="B4" t="s">
-        <v>613</v>
-      </c>
-      <c r="E4">
-        <v>1</v>
-      </c>
-      <c r="F4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="15">
-      <c r="A5" t="s">
-        <v>610</v>
-      </c>
-      <c r="B5" t="s">
-        <v>614</v>
-      </c>
-      <c r="E5">
-        <v>1</v>
-      </c>
-      <c r="F5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="15">
-      <c r="A6" t="s">
-        <v>615</v>
-      </c>
-      <c r="B6" t="s">
-        <v>616</v>
-      </c>
-      <c r="E6">
-        <v>49</v>
-      </c>
-      <c r="F6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="15">
-      <c r="A7" t="s">
-        <v>617</v>
-      </c>
-      <c r="B7" t="s">
-        <v>611</v>
-      </c>
-      <c r="E7">
-        <v>2</v>
-      </c>
-      <c r="F7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="15">
-      <c r="A8" t="s">
-        <v>617</v>
-      </c>
-      <c r="B8" t="s">
-        <v>612</v>
-      </c>
-      <c r="E8">
-        <v>126</v>
-      </c>
-      <c r="F8" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="15">
-      <c r="A9" t="s">
-        <v>617</v>
-      </c>
-      <c r="B9" t="s">
-        <v>613</v>
-      </c>
-      <c r="E9">
-        <v>28</v>
-      </c>
-      <c r="F9" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="15">
-      <c r="A10" t="s">
-        <v>617</v>
-      </c>
-      <c r="B10" t="s">
-        <v>614</v>
-      </c>
-      <c r="E10">
-        <v>22</v>
-      </c>
-      <c r="F10" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="15">
-      <c r="A11" t="s">
-        <v>618</v>
-      </c>
-      <c r="B11" t="s">
-        <v>619</v>
-      </c>
-      <c r="E11">
-        <v>3</v>
-      </c>
-      <c r="F11" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="15">
-      <c r="A12" t="s">
-        <v>618</v>
-      </c>
-      <c r="B12" t="s">
-        <v>620</v>
-      </c>
-      <c r="E12">
-        <v>17</v>
-      </c>
-      <c r="F12" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="15">
-      <c r="A13" t="s">
-        <v>618</v>
-      </c>
-      <c r="B13" t="s">
-        <v>621</v>
-      </c>
-      <c r="E13">
-        <v>88</v>
-      </c>
-      <c r="F13" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="15">
-      <c r="A14" t="s">
-        <v>618</v>
-      </c>
-      <c r="B14" t="s">
-        <v>622</v>
-      </c>
-      <c r="E14">
-        <v>13</v>
-      </c>
-      <c r="F14" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="15">
-      <c r="A15" t="s">
-        <v>618</v>
-      </c>
-      <c r="B15" t="s">
-        <v>623</v>
-      </c>
-      <c r="E15">
-        <v>6</v>
-      </c>
-      <c r="F15" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="15">
-      <c r="A16" t="s">
-        <v>618</v>
-      </c>
-      <c r="B16" t="s">
-        <v>614</v>
-      </c>
-      <c r="E16">
-        <v>6</v>
-      </c>
-      <c r="F16" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" ht="15">
-      <c r="A17" t="s">
-        <v>624</v>
-      </c>
-      <c r="B17" t="s">
-        <v>625</v>
-      </c>
-      <c r="E17">
-        <v>7</v>
-      </c>
-      <c r="F17" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" ht="15">
-      <c r="A18" t="s">
-        <v>624</v>
-      </c>
-      <c r="B18" t="s">
-        <v>626</v>
-      </c>
-      <c r="E18">
-        <v>14</v>
-      </c>
-      <c r="F18" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" ht="15">
-      <c r="A19" t="s">
-        <v>627</v>
-      </c>
-      <c r="B19" t="s">
-        <v>628</v>
-      </c>
-      <c r="E19">
-        <v>11</v>
-      </c>
-      <c r="F19" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" ht="15">
-      <c r="A20" t="s">
-        <v>627</v>
-      </c>
-      <c r="B20" t="s">
-        <v>629</v>
-      </c>
-      <c r="E20">
-        <v>1</v>
-      </c>
-      <c r="F20" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" ht="15">
-      <c r="A21" t="s">
-        <v>630</v>
-      </c>
-      <c r="B21" t="s">
-        <v>631</v>
-      </c>
-      <c r="E21">
-        <v>2</v>
-      </c>
-      <c r="F21" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" ht="15">
-      <c r="A22" t="s">
-        <v>632</v>
-      </c>
-      <c r="B22" t="s">
-        <v>633</v>
-      </c>
-      <c r="E22">
-        <v>4</v>
-      </c>
-      <c r="F22" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" ht="15">
-      <c r="A23" t="s">
-        <v>634</v>
-      </c>
-      <c r="B23" t="s">
-        <v>635</v>
-      </c>
-      <c r="E23">
-        <v>12</v>
-      </c>
-      <c r="F23" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" ht="15">
-      <c r="A24" t="s">
-        <v>636</v>
-      </c>
-      <c r="B24" t="s">
-        <v>637</v>
-      </c>
-      <c r="E24">
-        <v>10</v>
-      </c>
-      <c r="F24" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" ht="15">
-      <c r="A25" t="s">
-        <v>638</v>
-      </c>
-      <c r="B25" t="s">
-        <v>639</v>
-      </c>
-      <c r="E25">
-        <v>4</v>
-      </c>
-      <c r="F25" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" ht="15">
-      <c r="A26" t="s">
-        <v>640</v>
-      </c>
-      <c r="B26" t="s">
-        <v>641</v>
-      </c>
-      <c r="E26">
-        <v>2</v>
-      </c>
-      <c r="F26" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" ht="15">
-      <c r="A27" t="s">
-        <v>642</v>
-      </c>
-      <c r="B27" t="s">
-        <v>643</v>
-      </c>
-      <c r="E27">
-        <v>16</v>
-      </c>
-      <c r="F27" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" ht="15">
-      <c r="A28" t="s">
-        <v>642</v>
-      </c>
-      <c r="B28" t="s">
-        <v>644</v>
-      </c>
-      <c r="E28">
-        <v>4</v>
-      </c>
-      <c r="F28" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" ht="15">
-      <c r="A29" t="s">
-        <v>642</v>
-      </c>
-      <c r="B29" t="s">
-        <v>645</v>
-      </c>
-      <c r="E29">
-        <v>5</v>
-      </c>
-      <c r="F29" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" ht="15">
-      <c r="A30" t="s">
-        <v>646</v>
-      </c>
-      <c r="B30" t="s">
-        <v>647</v>
-      </c>
-      <c r="E30">
-        <v>6</v>
-      </c>
-      <c r="F30" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" ht="15">
-      <c r="A31" t="s">
-        <v>648</v>
-      </c>
-      <c r="B31" t="s">
-        <v>649</v>
-      </c>
-      <c r="E31">
-        <v>2</v>
-      </c>
-      <c r="F31" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" ht="15">
-      <c r="A32" t="s">
-        <v>650</v>
-      </c>
-      <c r="B32" t="s">
-        <v>651</v>
-      </c>
-      <c r="E32">
-        <v>4</v>
-      </c>
-      <c r="F32" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" ht="15">
-      <c r="A33" t="s">
-        <v>652</v>
-      </c>
-      <c r="B33" t="s">
-        <v>653</v>
-      </c>
-      <c r="E33">
-        <v>5</v>
-      </c>
-      <c r="F33" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" ht="15">
-      <c r="A34" t="s">
-        <v>654</v>
-      </c>
-      <c r="B34" t="s">
-        <v>655</v>
-      </c>
-      <c r="E34">
-        <v>12</v>
-      </c>
-      <c r="F34" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" ht="15">
-      <c r="A35" t="s">
-        <v>654</v>
-      </c>
-      <c r="B35" t="s">
-        <v>656</v>
-      </c>
-      <c r="E35">
-        <v>9</v>
-      </c>
-      <c r="F35" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" ht="15">
-      <c r="A36" t="s">
-        <v>654</v>
-      </c>
-      <c r="B36" t="s">
-        <v>657</v>
-      </c>
-      <c r="E36">
-        <v>6</v>
-      </c>
-      <c r="F36" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" ht="15">
-      <c r="A37" t="s">
-        <v>658</v>
-      </c>
-      <c r="B37" t="s">
-        <v>659</v>
-      </c>
-      <c r="E37">
-        <v>4</v>
-      </c>
-      <c r="F37" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" ht="15">
-      <c r="A38" t="s">
-        <v>658</v>
-      </c>
-      <c r="B38" t="s">
-        <v>660</v>
-      </c>
-      <c r="E38">
-        <v>3</v>
-      </c>
-      <c r="F38" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" ht="15">
-      <c r="A39" t="s">
-        <v>658</v>
-      </c>
-      <c r="B39" t="s">
-        <v>661</v>
-      </c>
-      <c r="E39">
-        <v>3</v>
-      </c>
-      <c r="F39" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" ht="15">
-      <c r="A40" t="s">
-        <v>658</v>
-      </c>
-      <c r="B40" t="s">
-        <v>662</v>
-      </c>
-      <c r="E40">
-        <v>1</v>
-      </c>
-      <c r="F40" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" ht="15">
-      <c r="A41" t="s">
-        <v>663</v>
-      </c>
-      <c r="B41" t="s">
-        <v>664</v>
-      </c>
-      <c r="E41">
-        <v>5</v>
-      </c>
-      <c r="F41" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" ht="15">
-      <c r="A42" t="s">
-        <v>663</v>
-      </c>
-      <c r="B42" t="s">
-        <v>665</v>
-      </c>
-      <c r="E42">
-        <v>1</v>
-      </c>
-      <c r="F42" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" ht="15">
-      <c r="A43" t="s">
-        <v>663</v>
-      </c>
-      <c r="B43" t="s">
-        <v>666</v>
-      </c>
-      <c r="E43">
-        <v>5</v>
-      </c>
-      <c r="F43" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" ht="15">
-      <c r="A44" t="s">
-        <v>667</v>
-      </c>
-      <c r="B44" t="s">
-        <v>668</v>
-      </c>
-      <c r="E44">
-        <v>3</v>
-      </c>
-      <c r="F44" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" ht="15">
-      <c r="A45" t="s">
-        <v>667</v>
-      </c>
-      <c r="B45" t="s">
-        <v>669</v>
-      </c>
-      <c r="E45">
-        <v>1</v>
-      </c>
-      <c r="F45" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" ht="15">
-      <c r="A46" t="s">
-        <v>667</v>
-      </c>
-      <c r="B46" t="s">
-        <v>670</v>
-      </c>
-      <c r="E46">
-        <v>12</v>
-      </c>
-      <c r="F46" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" ht="15">
-      <c r="A47" t="s">
-        <v>667</v>
-      </c>
-      <c r="B47" t="s">
-        <v>671</v>
-      </c>
-      <c r="E47">
-        <v>5421</v>
-      </c>
-      <c r="F47" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" ht="15">
-      <c r="A48" t="s">
-        <v>667</v>
-      </c>
-      <c r="B48" t="s">
-        <v>672</v>
-      </c>
-      <c r="E48">
-        <v>2</v>
-      </c>
-      <c r="F48" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" ht="15">
-      <c r="A49" t="s">
-        <v>667</v>
-      </c>
-      <c r="B49" t="s">
-        <v>673</v>
-      </c>
-      <c r="E49">
-        <v>360</v>
-      </c>
-      <c r="F49" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" ht="15">
-      <c r="A50" t="s">
-        <v>674</v>
-      </c>
-      <c r="B50" t="s">
-        <v>675</v>
-      </c>
-      <c r="E50">
-        <v>227</v>
-      </c>
-      <c r="F50" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" ht="15">
-      <c r="A51" t="s">
-        <v>674</v>
-      </c>
-      <c r="B51" t="s">
-        <v>676</v>
-      </c>
-      <c r="E51">
-        <v>899</v>
-      </c>
-      <c r="F51" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" ht="15">
-      <c r="A52" t="s">
-        <v>674</v>
-      </c>
-      <c r="B52" t="s">
-        <v>677</v>
-      </c>
-      <c r="E52">
-        <v>4</v>
-      </c>
-      <c r="F52" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" ht="15">
-      <c r="A53" t="s">
-        <v>674</v>
-      </c>
-      <c r="B53" t="s">
-        <v>678</v>
-      </c>
-      <c r="E53">
-        <v>12337</v>
-      </c>
-      <c r="F53" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" ht="15">
-      <c r="A54" t="s">
-        <v>679</v>
-      </c>
-      <c r="B54" t="s">
-        <v>680</v>
-      </c>
-      <c r="E54">
-        <v>501</v>
-      </c>
-      <c r="F54" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" ht="15">
-      <c r="A55" t="s">
-        <v>681</v>
-      </c>
-      <c r="B55" t="s">
-        <v>682</v>
-      </c>
-      <c r="E55">
-        <v>74</v>
-      </c>
-      <c r="F55" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6" ht="15">
-      <c r="A56" t="s">
-        <v>681</v>
-      </c>
-      <c r="B56" t="s">
-        <v>683</v>
-      </c>
-      <c r="E56">
-        <v>1</v>
-      </c>
-      <c r="F56" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6" ht="15">
-      <c r="A57" t="s">
-        <v>684</v>
-      </c>
-      <c r="B57" t="s">
-        <v>685</v>
-      </c>
-      <c r="E57">
-        <v>2</v>
-      </c>
-      <c r="F57" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6" ht="15">
-      <c r="A58" t="s">
-        <v>684</v>
-      </c>
-      <c r="B58" t="s">
-        <v>686</v>
-      </c>
-      <c r="E58">
-        <v>1</v>
-      </c>
-      <c r="F58" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6" ht="15">
-      <c r="A59" t="s">
-        <v>684</v>
-      </c>
-      <c r="B59" t="s">
-        <v>687</v>
-      </c>
-      <c r="E59">
-        <v>12</v>
-      </c>
-      <c r="F59" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6" ht="15">
-      <c r="A60" t="s">
-        <v>688</v>
-      </c>
-      <c r="B60" t="s">
-        <v>689</v>
-      </c>
-      <c r="E60">
-        <v>7</v>
-      </c>
-      <c r="F60" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6" ht="15">
-      <c r="A61" t="s">
-        <v>690</v>
-      </c>
-      <c r="B61" t="s">
-        <v>691</v>
-      </c>
-      <c r="E61">
-        <v>2</v>
-      </c>
-      <c r="F61" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="62" spans="1:6" ht="15">
-      <c r="A62" t="s">
-        <v>692</v>
-      </c>
-      <c r="B62" t="s">
-        <v>693</v>
-      </c>
-      <c r="E62">
-        <v>46</v>
-      </c>
-      <c r="F62" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="63" spans="1:6" ht="15">
-      <c r="A63" t="s">
-        <v>692</v>
-      </c>
-      <c r="B63" t="s">
-        <v>694</v>
-      </c>
-      <c r="E63">
-        <v>20</v>
-      </c>
-      <c r="F63" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="64" spans="1:6" ht="15">
-      <c r="A64" t="s">
-        <v>695</v>
-      </c>
-      <c r="B64" t="s">
-        <v>696</v>
-      </c>
-      <c r="E64">
-        <v>2</v>
-      </c>
-      <c r="F64" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="65" spans="1:6" ht="15">
-      <c r="A65" t="s">
-        <v>697</v>
-      </c>
-      <c r="B65" t="s">
-        <v>698</v>
-      </c>
-      <c r="E65">
-        <v>328</v>
-      </c>
-      <c r="F65" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="66" spans="1:6" ht="15">
-      <c r="A66" t="s">
-        <v>699</v>
-      </c>
-      <c r="B66" t="s">
-        <v>700</v>
-      </c>
-      <c r="E66">
-        <v>1</v>
-      </c>
-      <c r="F66" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="67" spans="1:6" ht="15">
-      <c r="A67" t="s">
-        <v>701</v>
-      </c>
-      <c r="B67" t="s">
-        <v>702</v>
-      </c>
-      <c r="E67">
-        <v>2</v>
-      </c>
-      <c r="F67" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="68" spans="1:6" ht="15">
-      <c r="A68" t="s">
-        <v>703</v>
-      </c>
-      <c r="B68" t="s">
-        <v>704</v>
-      </c>
-      <c r="E68">
-        <v>5</v>
-      </c>
-      <c r="F68" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="69" spans="1:6" ht="15">
-      <c r="A69" t="s">
-        <v>705</v>
-      </c>
-      <c r="B69" t="s">
-        <v>706</v>
-      </c>
-      <c r="E69">
-        <v>2</v>
-      </c>
-      <c r="F69" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="70" spans="1:6" ht="15">
-      <c r="A70" t="s">
-        <v>705</v>
-      </c>
-      <c r="B70" t="s">
-        <v>707</v>
-      </c>
-      <c r="E70">
-        <v>1</v>
-      </c>
-      <c r="F70" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="71" spans="1:6" ht="15">
-      <c r="A71" t="s">
-        <v>708</v>
-      </c>
-      <c r="B71" t="s">
-        <v>709</v>
-      </c>
-      <c r="E71">
-        <v>1</v>
-      </c>
-      <c r="F71" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="72" spans="1:6" ht="15"/>
-    <row r="73" spans="1:6" ht="15"/>
-    <row r="74" spans="1:6" ht="15"/>
-    <row r="75" spans="1:6" ht="15"/>
-    <row r="76" spans="1:6" ht="15"/>
-    <row r="77" spans="1:6" ht="15"/>
-    <row r="78" spans="1:6" ht="15"/>
-    <row r="79" spans="1:6" ht="15"/>
-    <row r="80" spans="1:6" ht="15"/>
+    <row r="73" spans="1:13" ht="15"/>
+    <row r="74" spans="1:13" ht="15"/>
+    <row r="75" spans="1:13" ht="15"/>
+    <row r="76" spans="1:13" ht="15"/>
+    <row r="77" spans="1:13" ht="15"/>
+    <row r="78" spans="1:13" ht="15"/>
+    <row r="79" spans="1:13" ht="15"/>
+    <row r="80" spans="1:13" ht="15"/>
     <row r="81" ht="15"/>
     <row r="82" ht="15"/>
     <row r="83" ht="15"/>

</xml_diff>